<commit_message>
QA test evidence for Week 7
</commit_message>
<xml_diff>
--- a/Harvey/Quality Assurance/QA Scripts.xlsx
+++ b/Harvey/Quality Assurance/QA Scripts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harvey\Desktop\FYP-IS484\Harvey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harvey\Desktop\FYP-IS484\Harvey\Quality Assurance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02617894-C601-40DC-8044-15496314954D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C10F845-CBBA-4DF7-8630-FB4DBF7F0DE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{73054CFE-414C-4BF5-89A7-9AB741DE9237}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="1" xr2:uid="{73054CFE-414C-4BF5-89A7-9AB741DE9237}"/>
   </bookViews>
   <sheets>
     <sheet name="QA Description" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>Use Case</t>
   </si>
@@ -223,12 +223,15 @@
   <si>
     <t>Week 13</t>
   </si>
+  <si>
+    <t>Completion Rate (%):</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +241,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -257,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -280,15 +290,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -299,18 +329,39 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -624,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7E952D8-DBC4-404B-B1AA-804BDD5A194B}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -640,198 +691,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="129" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="114.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="100.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="4">
+      <c r="A4" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="72" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="114.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="129" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="129" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="7">
+      <c r="A8" s="10">
         <v>3</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="171.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="5" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="72" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="171.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="5" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="129" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="5" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -855,77 +906,84 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C57DE9-8A69-4F45-BC20-47B1976F89C8}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="2"/>
-    <col min="2" max="2" width="32.19921875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.06640625" style="5"/>
+    <col min="2" max="2" width="32.19921875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="31.1328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.06640625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
@@ -934,15 +992,21 @@
       <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -951,21 +1015,27 @@
       <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="4">
+      <c r="A4" s="12">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -974,15 +1044,21 @@
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -991,15 +1067,21 @@
       <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -1008,15 +1090,21 @@
       <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -1025,21 +1113,27 @@
       <c r="M7" s="6"/>
     </row>
     <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="7">
+      <c r="A8" s="12">
         <v>3</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -1048,17 +1142,23 @@
       <c r="M8" s="6"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="5" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -1067,17 +1167,23 @@
       <c r="M9" s="6"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -1086,15 +1192,21 @@
       <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="5" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -1103,15 +1215,21 @@
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="5" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -1119,7 +1237,30 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:13" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="7">
+        <f>SUM(E2:E12)/COUNT(E2:E12)</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" ref="F13:G13" si="0">SUM(F2:F12)/COUNT(F2:F12)</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="7"/>
+    </row>
+    <row r="14" spans="1:13" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A8:A12"/>

</xml_diff>